<commit_message>
Updated relaatiotaulukko, names changed.
</commit_message>
<xml_diff>
--- a/Relaatio taulukko.xlsx
+++ b/Relaatio taulukko.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ville\workspace\Tietokannat-II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pilvi/git/Tietokannat-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13800" windowHeight="11660"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,75 +27,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>PELAAJA</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NIMI</t>
-  </si>
-  <si>
-    <t>PUHNUM</t>
-  </si>
-  <si>
-    <t>KOTIPAIKKA</t>
-  </si>
-  <si>
     <t>RATA</t>
   </si>
   <si>
-    <t>LUOKITUS</t>
-  </si>
-  <si>
-    <t>VAYLIEN_LKM</t>
-  </si>
-  <si>
-    <t>OSOITE</t>
-  </si>
-  <si>
-    <t>RATAMESTARI</t>
-  </si>
-  <si>
     <t>PELI</t>
   </si>
   <si>
-    <t>RADAN_ID</t>
-  </si>
-  <si>
-    <t>PAIVAMAARA</t>
-  </si>
-  <si>
     <t>PELAAMASSA</t>
   </si>
   <si>
-    <t>PELIID</t>
-  </si>
-  <si>
-    <t>PELAAJAID</t>
-  </si>
-  <si>
     <t>SUORITUS</t>
   </si>
   <si>
-    <t>RADANID</t>
-  </si>
-  <si>
-    <t>VAYLANUMERO</t>
-  </si>
-  <si>
     <t>VAYLA</t>
   </si>
   <si>
-    <t>PAR</t>
-  </si>
-  <si>
-    <t>NUMERO</t>
-  </si>
-  <si>
-    <t>PITUUS</t>
+    <t>pelaajan_id</t>
+  </si>
+  <si>
+    <t>nimi</t>
+  </si>
+  <si>
+    <t>puhnum</t>
+  </si>
+  <si>
+    <t>kotipaikka</t>
+  </si>
+  <si>
+    <t>radan_id</t>
+  </si>
+  <si>
+    <t>luokitus</t>
+  </si>
+  <si>
+    <t>vaylien_lkm</t>
+  </si>
+  <si>
+    <t>osoite</t>
+  </si>
+  <si>
+    <t>ratamestari</t>
+  </si>
+  <si>
+    <t>pelin_id</t>
+  </si>
+  <si>
+    <t>paivamaara</t>
+  </si>
+  <si>
+    <t>vaylannumero</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>pituus</t>
   </si>
 </sst>
 </file>
@@ -142,16 +139,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -166,7 +163,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -182,7 +179,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -227,9 +224,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -262,9 +259,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -446,191 +443,191 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>

</xml_diff>

<commit_message>
Lisäsin tietokantaan yhden pelin
</commit_message>
<xml_diff>
--- a/Relaatio taulukko.xlsx
+++ b/Relaatio taulukko.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pilvi/git/Tietokannat-II/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ville\workspace\Tietokannat-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,18 +16,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>PELAAJA</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>pituus</t>
+  </si>
+  <si>
+    <t>heittojen_lkm</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -443,26 +446,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -476,24 +479,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -510,26 +513,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -540,22 +543,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -563,20 +566,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
@@ -589,25 +592,30 @@
       <c r="E24" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
@@ -621,13 +629,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>

</xml_diff>